<commit_message>
Corregir MER, MR, y Diccionario
</commit_message>
<xml_diff>
--- a/Documentos/Diccionario de Datos.xlsx
+++ b/Documentos/Diccionario de Datos.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="78">
   <si>
     <t>DICCIONARIO DE DATOS</t>
   </si>
@@ -148,118 +148,97 @@
     <t>Nombre del proveedor del producto</t>
   </si>
   <si>
+    <t>Inventario</t>
+  </si>
+  <si>
+    <t>Registro de las ventas realizadas</t>
+  </si>
+  <si>
+    <t>FK</t>
+  </si>
+  <si>
+    <t>NombreProducto</t>
+  </si>
+  <si>
+    <t>Varchar (50)</t>
+  </si>
+  <si>
+    <t>Nombre identificador de producto en inventario</t>
+  </si>
+  <si>
+    <t>Cantidad</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>Número de cantidad de producto en almacen</t>
+  </si>
+  <si>
+    <t>fechaDeREgistro</t>
+  </si>
+  <si>
+    <t>Ultima hora de modificacion en inventario</t>
+  </si>
+  <si>
+    <t>Relaciones</t>
+  </si>
+  <si>
+    <t>Compra</t>
+  </si>
+  <si>
+    <t>Descripcion:</t>
+  </si>
+  <si>
+    <t>Registro de las compras de los productos</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Número identificador de la compra</t>
+  </si>
+  <si>
+    <t>Nombre de producto comprado</t>
+  </si>
+  <si>
+    <t>fecha y hora en la que se registro la compra</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>El total que se registro en la compra</t>
+  </si>
+  <si>
+    <t>Precio al que se compró una unidad de producto</t>
+  </si>
+  <si>
+    <t>cantidad</t>
+  </si>
+  <si>
+    <t>cantidad de producto que se compro</t>
+  </si>
+  <si>
     <t>Venta</t>
   </si>
   <si>
-    <t>Descripcion:</t>
-  </si>
-  <si>
-    <t>Registro de las ventas realizadas</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>double</t>
+    <t>Registro de la venta de los productos</t>
   </si>
   <si>
     <t>Número identificador de la venta</t>
   </si>
   <si>
+    <t>Nombre de producto vendido</t>
+  </si>
+  <si>
     <t>fecha y hora en la que se registro la venta</t>
   </si>
   <si>
-    <t>total</t>
-  </si>
-  <si>
     <t>La suma total de precios de venta</t>
   </si>
   <si>
-    <t>FK</t>
-  </si>
-  <si>
-    <t>Nombre de la cuenta de usaurio que realizo la venta</t>
-  </si>
-  <si>
-    <t>Compra</t>
-  </si>
-  <si>
-    <t>Registro de las compras de los productos</t>
-  </si>
-  <si>
-    <t>Número identificador de la compra</t>
-  </si>
-  <si>
-    <t>fecha y hora en la que se registro la compra</t>
-  </si>
-  <si>
-    <t>El total que se registro en la compra</t>
-  </si>
-  <si>
-    <t>Nombre de la cuenta de usuario que realizo la compra</t>
-  </si>
-  <si>
-    <t>Inventario</t>
-  </si>
-  <si>
-    <t>NombreProducto</t>
-  </si>
-  <si>
-    <t>Varchar (50)</t>
-  </si>
-  <si>
-    <t>Nombre identificador de producto en inventario</t>
-  </si>
-  <si>
-    <t>Cantidad</t>
-  </si>
-  <si>
-    <t>int</t>
-  </si>
-  <si>
-    <t>Número de cantidad de producto en almacen</t>
-  </si>
-  <si>
-    <t>fechaDeREgistro</t>
-  </si>
-  <si>
-    <t>Ultima hora de modificacion en inventario</t>
-  </si>
-  <si>
-    <t>Relaciones</t>
-  </si>
-  <si>
-    <t>Compra_Producto</t>
-  </si>
-  <si>
-    <t>idCompra</t>
-  </si>
-  <si>
-    <t>Nombre de producto comprado</t>
-  </si>
-  <si>
-    <t>PrecioCompra</t>
-  </si>
-  <si>
-    <t>Precio al que se compró una unidad de producto</t>
-  </si>
-  <si>
-    <t>cantidad</t>
-  </si>
-  <si>
-    <t>cantidad de producto que se compro</t>
-  </si>
-  <si>
-    <t>Venta_Producto</t>
-  </si>
-  <si>
-    <t>idVenta</t>
-  </si>
-  <si>
-    <t>Número identificador de la centa</t>
-  </si>
-  <si>
-    <t>Nombre de producto vendido</t>
+    <t>precioVenta</t>
   </si>
   <si>
     <t>Precio al que se vendió una unidad de producto</t>
@@ -272,7 +251,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -300,13 +279,6 @@
       <name val="Arial"/>
     </font>
     <font/>
-    <font>
-      <b/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -316,7 +288,7 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="17">
     <border/>
     <border>
       <bottom style="thick">
@@ -394,6 +366,50 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -424,7 +440,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="36">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -478,30 +494,45 @@
     <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="9" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="11" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="12" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="13" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="13" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="14" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="15" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="16" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -1135,10 +1166,10 @@
     </row>
     <row r="30">
       <c r="A30" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>47</v>
       </c>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
@@ -1178,19 +1209,19 @@
       <c r="H32" s="2"/>
     </row>
     <row r="33">
-      <c r="A33" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B33" s="17" t="s">
+      <c r="A33" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="C33" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D33" s="17" t="s">
+      <c r="C33" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="E33" s="7" t="s">
+      <c r="E33" s="23" t="s">
         <v>50</v>
       </c>
       <c r="F33" s="8"/>
@@ -1199,704 +1230,503 @@
     </row>
     <row r="34">
       <c r="A34" s="18"/>
-      <c r="B34" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C34" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D34" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="E34" s="7" t="s">
+      <c r="B34" s="22" t="s">
         <v>51</v>
+      </c>
+      <c r="C34" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="E34" s="23" t="s">
+        <v>53</v>
       </c>
       <c r="F34" s="8"/>
       <c r="G34" s="9"/>
       <c r="H34" s="2"/>
     </row>
     <row r="35">
-      <c r="A35" s="21"/>
-      <c r="B35" s="17" t="s">
+      <c r="A35" s="19"/>
+      <c r="B35" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="C35" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E35" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="F35" s="11"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="2"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="4"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="2"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="2"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="2"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="10"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="2"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F43" s="11"/>
+      <c r="G43" s="12"/>
+      <c r="H43" s="2"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B44" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C44" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D44" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D35" s="17" t="s">
+      <c r="E44" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F44" s="11"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="2"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B45" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D45" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E45" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F45" s="30"/>
+      <c r="G45" s="31"/>
+      <c r="H45" s="2"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C46" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D46" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F46" s="8"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="2"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="18"/>
+      <c r="B47" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C47" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D47" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F47" s="8"/>
+      <c r="G47" s="9"/>
+      <c r="H47" s="2"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="32"/>
+      <c r="B48" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C48" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D48" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="E35" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="F35" s="8"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="2"/>
-    </row>
-    <row r="36">
-      <c r="A36" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="B36" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="C36" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="D36" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F36" s="11"/>
-      <c r="G36" s="12"/>
-      <c r="H36" s="2"/>
-    </row>
-    <row r="37">
-      <c r="A37" s="4"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="2"/>
-    </row>
-    <row r="38">
-      <c r="A38" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="2"/>
-    </row>
-    <row r="39">
-      <c r="A39" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="2"/>
-    </row>
-    <row r="40">
-      <c r="A40" s="10"/>
-      <c r="B40" s="11"/>
-      <c r="C40" s="11"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="12"/>
-      <c r="H40" s="2"/>
-    </row>
-    <row r="41">
-      <c r="A41" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B41" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C41" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D41" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E41" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="F41" s="11"/>
-      <c r="G41" s="12"/>
-      <c r="H41" s="2"/>
-    </row>
-    <row r="42">
-      <c r="A42" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B42" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="C42" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D42" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="F42" s="8"/>
-      <c r="G42" s="9"/>
-      <c r="H42" s="2"/>
-    </row>
-    <row r="43">
-      <c r="A43" s="18"/>
-      <c r="B43" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C43" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D43" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F43" s="8"/>
-      <c r="G43" s="9"/>
-      <c r="H43" s="2"/>
-    </row>
-    <row r="44">
-      <c r="A44" s="21"/>
-      <c r="B44" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="C44" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D44" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="E44" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="F44" s="8"/>
-      <c r="G44" s="9"/>
-      <c r="H44" s="2"/>
-    </row>
-    <row r="45">
-      <c r="A45" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="B45" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="C45" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="D45" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="F45" s="11"/>
-      <c r="G45" s="12"/>
-      <c r="H45" s="2"/>
-    </row>
-    <row r="46">
-      <c r="A46" s="2"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
-    </row>
-    <row r="47">
-      <c r="A47" s="4"/>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
-      <c r="H47" s="2"/>
-    </row>
-    <row r="48">
-      <c r="A48" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B48" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C48" s="8"/>
-      <c r="D48" s="8"/>
-      <c r="E48" s="8"/>
+      <c r="E48" s="7" t="s">
+        <v>65</v>
+      </c>
       <c r="F48" s="8"/>
       <c r="G48" s="9"/>
       <c r="H48" s="2"/>
     </row>
     <row r="49">
-      <c r="A49" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B49" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C49" s="8"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="8"/>
+      <c r="A49" s="32"/>
+      <c r="B49" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C49" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D49" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>66</v>
+      </c>
       <c r="F49" s="8"/>
       <c r="G49" s="9"/>
       <c r="H49" s="2"/>
     </row>
     <row r="50">
-      <c r="A50" s="10"/>
-      <c r="B50" s="11"/>
-      <c r="C50" s="11"/>
-      <c r="D50" s="11"/>
-      <c r="E50" s="11"/>
+      <c r="A50" s="33"/>
+      <c r="B50" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="C50" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D50" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>68</v>
+      </c>
       <c r="F50" s="11"/>
       <c r="G50" s="12"/>
       <c r="H50" s="2"/>
     </row>
     <row r="51">
-      <c r="A51" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B51" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C51" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D51" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E51" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="F51" s="11"/>
-      <c r="G51" s="12"/>
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
     <row r="52">
-      <c r="A52" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="B52" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="C52" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D52" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="E52" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="F52" s="8"/>
-      <c r="G52" s="9"/>
+      <c r="A52" s="4"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
       <c r="H52" s="2"/>
     </row>
     <row r="53">
-      <c r="A53" s="18"/>
-      <c r="B53" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="C53" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D53" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="E53" s="25" t="s">
-        <v>68</v>
-      </c>
+      <c r="A53" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B53" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="C53" s="8"/>
+      <c r="D53" s="8"/>
+      <c r="E53" s="8"/>
       <c r="F53" s="8"/>
       <c r="G53" s="9"/>
       <c r="H53" s="2"/>
     </row>
     <row r="54">
-      <c r="A54" s="19"/>
+      <c r="A54" s="6" t="s">
+        <v>58</v>
+      </c>
       <c r="B54" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="C54" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="D54" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="C54" s="8"/>
+      <c r="D54" s="8"/>
+      <c r="E54" s="8"/>
+      <c r="F54" s="8"/>
+      <c r="G54" s="9"/>
+      <c r="H54" s="2"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="10"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="11"/>
+      <c r="E55" s="11"/>
+      <c r="F55" s="11"/>
+      <c r="G55" s="12"/>
+      <c r="H55" s="2"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B56" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D56" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E56" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F56" s="11"/>
+      <c r="G56" s="12"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B57" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C57" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D57" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="E57" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="F57" s="11"/>
+      <c r="G57" s="12"/>
+      <c r="H57" s="35"/>
+      <c r="I57" s="35"/>
+      <c r="J57" s="35"/>
+      <c r="K57" s="35"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B58" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C58" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D58" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E58" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F58" s="8"/>
+      <c r="G58" s="9"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B59" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C59" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D59" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E54" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="F54" s="11"/>
-      <c r="G54" s="12"/>
-      <c r="H54" s="2"/>
-    </row>
-    <row r="55">
-      <c r="A55" s="2"/>
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
-      <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
-      <c r="G55" s="2"/>
-      <c r="H55" s="2"/>
-    </row>
-    <row r="56">
-      <c r="A56" s="2"/>
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
-      <c r="G56" s="2"/>
-      <c r="H56" s="2"/>
-    </row>
-    <row r="57">
-      <c r="A57" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
-      <c r="D57" s="2"/>
-      <c r="E57" s="2"/>
-      <c r="F57" s="2"/>
-      <c r="G57" s="2"/>
-      <c r="H57" s="2"/>
-    </row>
-    <row r="58">
-      <c r="A58" s="4"/>
-      <c r="B58" s="5"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="5"/>
-      <c r="E58" s="5"/>
-      <c r="F58" s="5"/>
-      <c r="G58" s="5"/>
-      <c r="H58" s="2"/>
-    </row>
-    <row r="59">
-      <c r="A59" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B59" s="7" t="s">
+      <c r="E59" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C59" s="8"/>
-      <c r="D59" s="8"/>
-      <c r="E59" s="8"/>
       <c r="F59" s="8"/>
       <c r="G59" s="9"/>
-      <c r="H59" s="2"/>
     </row>
     <row r="60">
-      <c r="A60" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B60" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C60" s="8"/>
-      <c r="D60" s="8"/>
-      <c r="E60" s="8"/>
+      <c r="A60" s="18"/>
+      <c r="B60" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C60" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D60" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="F60" s="8"/>
       <c r="G60" s="9"/>
-      <c r="H60" s="2"/>
     </row>
     <row r="61">
-      <c r="A61" s="10"/>
-      <c r="B61" s="11"/>
-      <c r="C61" s="11"/>
-      <c r="D61" s="11"/>
-      <c r="E61" s="11"/>
-      <c r="F61" s="11"/>
-      <c r="G61" s="12"/>
+      <c r="A61" s="32"/>
+      <c r="B61" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D61" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E61" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F61" s="8"/>
+      <c r="G61" s="9"/>
       <c r="H61" s="2"/>
     </row>
     <row r="62">
-      <c r="A62" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B62" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C62" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D62" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E62" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="F62" s="11"/>
-      <c r="G62" s="12"/>
+      <c r="A62" s="32"/>
+      <c r="B62" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="C62" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D62" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E62" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F62" s="8"/>
+      <c r="G62" s="9"/>
       <c r="H62" s="2"/>
     </row>
     <row r="63">
-      <c r="A63" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="B63" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="C63" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D63" s="17" t="s">
-        <v>49</v>
+      <c r="A63" s="33"/>
+      <c r="B63" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="C63" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D63" s="20" t="s">
+        <v>52</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F63" s="11"/>
       <c r="G63" s="12"/>
       <c r="H63" s="2"/>
     </row>
     <row r="64">
-      <c r="A64" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="B64" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="C64" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D64" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="E64" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="F64" s="8"/>
-      <c r="G64" s="9"/>
+      <c r="A64" s="2"/>
+      <c r="B64" s="2"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+      <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
     <row r="65">
-      <c r="A65" s="21"/>
-      <c r="B65" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="C65" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D65" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="E65" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="F65" s="8"/>
-      <c r="G65" s="9"/>
+      <c r="A65" s="2"/>
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66">
-      <c r="A66" s="22"/>
-      <c r="B66" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="C66" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="D66" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="E66" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="F66" s="11"/>
-      <c r="G66" s="12"/>
-      <c r="H66" s="2"/>
-    </row>
-    <row r="67">
-      <c r="A67" s="2"/>
-      <c r="B67" s="2"/>
-      <c r="C67" s="2"/>
-      <c r="D67" s="2"/>
-      <c r="E67" s="2"/>
-      <c r="F67" s="2"/>
-      <c r="G67" s="2"/>
-      <c r="H67" s="2"/>
-    </row>
-    <row r="68">
-      <c r="A68" s="4"/>
-      <c r="B68" s="5"/>
-      <c r="C68" s="5"/>
-      <c r="D68" s="5"/>
-      <c r="E68" s="5"/>
-      <c r="F68" s="5"/>
-      <c r="G68" s="5"/>
-      <c r="H68" s="2"/>
-    </row>
-    <row r="69">
-      <c r="A69" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B69" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C69" s="8"/>
-      <c r="D69" s="8"/>
-      <c r="E69" s="8"/>
-      <c r="F69" s="8"/>
-      <c r="G69" s="9"/>
-      <c r="H69" s="2"/>
-    </row>
-    <row r="70">
-      <c r="A70" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B70" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C70" s="8"/>
-      <c r="D70" s="8"/>
-      <c r="E70" s="8"/>
-      <c r="F70" s="8"/>
-      <c r="G70" s="9"/>
-      <c r="H70" s="2"/>
-    </row>
-    <row r="71">
-      <c r="A71" s="10"/>
-      <c r="B71" s="11"/>
-      <c r="C71" s="11"/>
-      <c r="D71" s="11"/>
-      <c r="E71" s="11"/>
-      <c r="F71" s="11"/>
-      <c r="G71" s="12"/>
-      <c r="H71" s="2"/>
-    </row>
-    <row r="72">
-      <c r="A72" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B72" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C72" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D72" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E72" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="F72" s="11"/>
-      <c r="G72" s="12"/>
-      <c r="H72" s="2"/>
-    </row>
-    <row r="73">
-      <c r="A73" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="B73" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="C73" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D73" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="E73" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F73" s="11"/>
-      <c r="G73" s="12"/>
-      <c r="H73" s="2"/>
-    </row>
-    <row r="74">
-      <c r="A74" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="B74" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="C74" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D74" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="E74" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="F74" s="8"/>
-      <c r="G74" s="9"/>
-      <c r="H74" s="2"/>
-    </row>
-    <row r="75">
-      <c r="A75" s="21"/>
-      <c r="B75" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="C75" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D75" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="E75" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="F75" s="8"/>
-      <c r="G75" s="9"/>
-      <c r="H75" s="2"/>
-    </row>
-    <row r="76">
-      <c r="A76" s="22"/>
-      <c r="B76" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="C76" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="D76" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="E76" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="F76" s="11"/>
-      <c r="G76" s="12"/>
-      <c r="H76" s="2"/>
-    </row>
-    <row r="77">
-      <c r="A77" s="2"/>
-      <c r="B77" s="2"/>
-      <c r="C77" s="2"/>
-      <c r="D77" s="2"/>
-      <c r="E77" s="2"/>
-      <c r="F77" s="2"/>
-      <c r="G77" s="2"/>
-      <c r="H77" s="2"/>
-    </row>
-    <row r="78">
-      <c r="A78" s="2"/>
-      <c r="B78" s="2"/>
-      <c r="C78" s="2"/>
-      <c r="D78" s="2"/>
-      <c r="E78" s="2"/>
-      <c r="F78" s="2"/>
-      <c r="G78" s="2"/>
-      <c r="H78" s="2"/>
-    </row>
   </sheetData>
-  <mergeCells count="59">
-    <mergeCell ref="E54:G54"/>
-    <mergeCell ref="B59:G59"/>
-    <mergeCell ref="B60:G60"/>
-    <mergeCell ref="A61:G61"/>
-    <mergeCell ref="E62:G62"/>
-    <mergeCell ref="E63:G63"/>
-    <mergeCell ref="E64:G64"/>
-    <mergeCell ref="E65:G65"/>
-    <mergeCell ref="E66:G66"/>
-    <mergeCell ref="B69:G69"/>
-    <mergeCell ref="B70:G70"/>
-    <mergeCell ref="A71:G71"/>
-    <mergeCell ref="E72:G72"/>
-    <mergeCell ref="E73:G73"/>
+  <mergeCells count="49">
     <mergeCell ref="A1:F2"/>
     <mergeCell ref="B6:G6"/>
     <mergeCell ref="B7:G7"/>
@@ -1924,24 +1754,28 @@
     <mergeCell ref="E33:G33"/>
     <mergeCell ref="E34:G34"/>
     <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="B39:G39"/>
-    <mergeCell ref="A40:G40"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="B41:G41"/>
+    <mergeCell ref="A42:G42"/>
     <mergeCell ref="E43:G43"/>
     <mergeCell ref="E44:G44"/>
     <mergeCell ref="E45:G45"/>
-    <mergeCell ref="B48:G48"/>
-    <mergeCell ref="B49:G49"/>
-    <mergeCell ref="A50:G50"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="E74:G74"/>
-    <mergeCell ref="E75:G75"/>
-    <mergeCell ref="E76:G76"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="E56:G56"/>
+    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="E59:G59"/>
+    <mergeCell ref="E60:G60"/>
+    <mergeCell ref="E61:G61"/>
+    <mergeCell ref="E62:G62"/>
+    <mergeCell ref="E63:G63"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="B53:G53"/>
+    <mergeCell ref="B54:G54"/>
+    <mergeCell ref="A55:G55"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>